<commit_message>
Extraordinary overwrite: New v1 version
</commit_message>
<xml_diff>
--- a/dandem_demens_v100_export.xlsx
+++ b/dandem_demens_v100_export.xlsx
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="34" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
     <col width="46" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
@@ -488,12 +488,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RUDAS</t>
+          <t>ExtendedNeuroAssessment</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -505,12 +505,12 @@
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -520,19 +520,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MCE</t>
+          <t>NPHAssessment</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -544,41 +544,51 @@
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Diagnosis</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Trinvold_DSQIID</t>
+          <t>EtiologicalDiagnosis</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Se webservice dokumentation.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>DiagnosisCode</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -586,9 +596,19 @@
           <t>str, Enum</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "alzheimer_sygdom" | "lewy_body_sygdom" | "parkinson_sygdom" | "cerebrovaskulaer_sygdom" | "mixed_alzheimer_cerebrovaskulaer" | "frontotemporal_demens" | "atypisk_parkinson_msa_cbs_psp" | "normaltryks_hydrocephalus_nph" | "huntingtons_sygdom" | "alkohol" | "anden_specifik_neurodegenerativ_sygdom" | "anden_ikke_neurodegenerativ_sygdom" | "psykiatrisk_sygdom" | "uafklaret_aetiologi" | "ikke_relevant" | </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -600,7 +620,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ADSC_ADL</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -622,7 +642,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 78</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 40</t>
         </is>
       </c>
     </row>
@@ -634,7 +654,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CAMcog</t>
+          <t>ACE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -656,7 +676,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 105</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
     </row>
@@ -668,7 +688,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MoCa</t>
+          <t>MMSE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -702,7 +722,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ACE</t>
+          <t>RUDAS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -722,9 +742,14 @@
           <t>Integer</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
         </is>
       </c>
     </row>
@@ -736,7 +761,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>FAQ_IADL</t>
+          <t>ADSC_ADL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -758,7 +783,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 78</t>
         </is>
       </c>
     </row>
@@ -770,7 +795,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>MoCa</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -792,7 +817,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 40</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
         </is>
       </c>
     </row>
@@ -804,17 +829,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CognitiveImpairment</t>
+          <t>MCE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>Se webservice dokumentation.</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>True</t>
         </is>
       </c>
     </row>
@@ -826,22 +846,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "kognitiv_intakt" | "kognitiv_svaekkelse" | "demens_let_grad" | "demens_moderat_grad" | "demens_svaer_grad" | </t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
     </row>
@@ -853,19 +863,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SupportPersonPresent</t>
+          <t>CognitiveImpairment</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>Se webservice dokumentation.</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -880,7 +895,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "habituel_kognitiv_funktion" | "kognitiv_svaekkelse" | "demens_let_grad" | "demens_moderat_grad" | "demens_svaer_grad" | </t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -892,7 +912,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MMSE</t>
+          <t>Trinvold</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -904,17 +924,17 @@
     <row r="25">
       <c r="D25" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>
@@ -926,7 +946,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BASIC</t>
+          <t>SupportPersonPresent</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -938,29 +958,34 @@
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 25</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>NPHAssessment</t>
+          <t>DSQIID</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -972,34 +997,29 @@
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ExtendedNeuroAssessment</t>
+          <t>CAMcog</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1011,120 +1031,85 @@
     <row r="31">
       <c r="D31" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 105</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>EtiologicalDiagnosis</t>
+          <t>BASIC</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>Se webservice dokumentation.</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>True</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>DiagnosisCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "alzheimer_sygdom" | "lewy_body_sygdom" | "parkinson_sygdom" | "cerebrovaskulaer_sygdom" | "mixed_alzheimer_cerebrovaskulaer" | "frontotemporal_demens" | "atypisk_parkinson_msa_cbs_psp" | "normaltryks_hydrocephalus_nph" | "huntingtons_sygdom" | "alkohol" | "anden_specifik_neurodegenerativ_sygdom" | "anden_ikke_neurodegenerativ_sygdom" | "psykiatrisk_sygdom" | "uafklaret_aetiologi" | "ikke_relevant" | </t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 25</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>InformDiagnosis</t>
+          <t>FAQ_IADL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>Se webservice dokumentation.</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>True</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
         </is>
       </c>
     </row>
@@ -1136,13 +1121,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ReferralFreeChoice</t>
+          <t>InformDiagnosis</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fritvalgshenvisning modtaget
-</t>
+          <t>Se webservice dokumentation.</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -1167,6 +1156,11 @@
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1176,7 +1170,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ReferralCommunalCoordinator</t>
+          <t>MunicipalDementiaCoordinator</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">

</xml_diff>